<commit_message>
feat(results): add results readme and plots
</commit_message>
<xml_diff>
--- a/hyperXGB/logs/all_datasets_comparison/comparison_results.xlsx
+++ b/hyperXGB/logs/all_datasets_comparison/comparison_results.xlsx
@@ -585,22 +585,22 @@
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>180.768278870758</v>
+        <v>186.6960269479135</v>
       </c>
       <c r="I2" t="n">
-        <v>35.57515001296997</v>
+        <v>31.60971188545227</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7037508487701416</v>
+        <v>0.6250641345977783</v>
       </c>
       <c r="M2" t="n">
-        <v>50.55077386427351</v>
+        <v>50.57034972226132</v>
       </c>
       <c r="N2" t="n">
         <v>1.948093995367479e-07</v>
@@ -609,31 +609,31 @@
         <v>3.195353716989785e-08</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9947634415149486</v>
+        <v>0.994824331729891</v>
       </c>
       <c r="Q2" t="n">
         <v>0.994824331729891</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9722421331832347</v>
+        <v>0.9725808417383324</v>
       </c>
       <c r="S2" t="n">
         <v>0.972355844896478</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9947634415149486</v>
+        <v>0.994824331729891</v>
       </c>
       <c r="U2" t="n">
         <v>0.994824331729891</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9657534347473216</v>
+        <v>0.9658255928677748</v>
       </c>
       <c r="W2" t="n">
         <v>0.9693307568571838</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9789368214266921</v>
+        <v>0.9795594864329188</v>
       </c>
       <c r="Y2" t="n">
         <v>0.9754249030922773</v>
@@ -664,58 +664,58 @@
         <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>593.4894865463432</v>
+        <v>537.8993470910575</v>
       </c>
       <c r="I3" t="n">
-        <v>24.76710104942322</v>
+        <v>35.9458270072937</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4451160430908203</v>
+        <v>0.6741127967834473</v>
       </c>
       <c r="M3" t="n">
-        <v>55.64189706002082</v>
+        <v>53.32316368834781</v>
       </c>
       <c r="N3" t="n">
-        <v>4.115399316766471e-08</v>
+        <v>0.001579694065001903</v>
       </c>
       <c r="O3" t="n">
-        <v>0.02573614257139147</v>
+        <v>0.02562779079587741</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9929367350666748</v>
+        <v>0.9938500882908117</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8994093649150582</v>
+        <v>0.9943981002252938</v>
       </c>
       <c r="R3" t="n">
-        <v>0.9613896818753057</v>
+        <v>0.9667621574284866</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6984370762348266</v>
+        <v>0.969813609955933</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9929367350666748</v>
+        <v>0.9938500882908117</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8994093649150582</v>
+        <v>0.9943981002252938</v>
       </c>
       <c r="V3" t="n">
-        <v>0.969312289728874</v>
+        <v>0.9692731960366257</v>
       </c>
       <c r="W3" t="n">
-        <v>0.649831906210916</v>
+        <v>0.97092948366718</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9537596688474559</v>
+        <v>0.9642809534667531</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.8756498517881887</v>
+        <v>0.9687036289968954</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +743,10 @@
         <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>1960.769972272889</v>
+        <v>1594.280011506716</v>
       </c>
       <c r="I4" t="n">
-        <v>67.56262302398682</v>
+        <v>69.56055402755737</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -755,10 +755,10 @@
         <v>4</v>
       </c>
       <c r="L4" t="n">
-        <v>1.084843158721924</v>
+        <v>1.209961891174316</v>
       </c>
       <c r="M4" t="n">
-        <v>62.27870128580037</v>
+        <v>57.48987181740581</v>
       </c>
       <c r="N4" t="n">
         <v>0.3080625870352865</v>
@@ -822,10 +822,10 @@
         <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>53.27744807121661</v>
+        <v>49.41097724230254</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4885706901550293</v>
+        <v>0.4972898960113525</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -834,10 +834,10 @@
         <v>100</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2377490997314453</v>
+        <v>0.2443199157714844</v>
       </c>
       <c r="M5" t="n">
-        <v>2.054984396184486</v>
+        <v>2.03540466376255</v>
       </c>
       <c r="N5" t="n">
         <v>8.590505752911891e-08</v>
@@ -901,10 +901,10 @@
         <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>149.0185792349727</v>
+        <v>138.1121856866538</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9193789958953857</v>
+        <v>0.9521069526672363</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -913,46 +913,46 @@
         <v>100</v>
       </c>
       <c r="L6" t="n">
-        <v>0.08474588394165039</v>
+        <v>0.08733320236206055</v>
       </c>
       <c r="M6" t="n">
-        <v>10.84865663243776</v>
+        <v>10.90200435706057</v>
       </c>
       <c r="N6" t="n">
-        <v>1.837292740700852e-08</v>
+        <v>0.001431014891680268</v>
       </c>
       <c r="O6" t="n">
-        <v>0.02786771828041146</v>
+        <v>0.02811760991289549</v>
       </c>
       <c r="P6" t="n">
         <v>0.8476190476190476</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.780952380952381</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="R6" t="n">
         <v>0.6022813165670309</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5595058536235007</v>
+        <v>0.5915966386554622</v>
       </c>
       <c r="T6" t="n">
         <v>0.8476190476190476</v>
       </c>
       <c r="U6" t="n">
-        <v>0.780952380952381</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="V6" t="n">
         <v>0.5672727272727273</v>
       </c>
       <c r="W6" t="n">
-        <v>0.5523809523809523</v>
+        <v>0.5634920634920635</v>
       </c>
       <c r="X6" t="n">
         <v>0.6462585034013606</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.5900965037177661</v>
+        <v>0.6288561936402468</v>
       </c>
     </row>
     <row r="7">
@@ -980,10 +980,10 @@
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>503.8680078508341</v>
+        <v>406.3967264224473</v>
       </c>
       <c r="I7" t="n">
-        <v>5.274669170379639</v>
+        <v>5.503466844558716</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -992,10 +992,10 @@
         <v>100</v>
       </c>
       <c r="L7" t="n">
-        <v>0.242556095123291</v>
+        <v>0.2481122016906738</v>
       </c>
       <c r="M7" t="n">
-        <v>21.74618274464936</v>
+        <v>22.18136313755335</v>
       </c>
       <c r="N7" t="n">
         <v>0.2805947281718134</v>
@@ -1264,10 +1264,10 @@
         <v>2</v>
       </c>
       <c r="H13" t="n">
-        <v>184.4349376114082</v>
+        <v>155.3291394061399</v>
       </c>
       <c r="I13" t="n">
-        <v>2.297486782073975</v>
+        <v>2.278520107269287</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -1276,10 +1276,10 @@
         <v>100</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2540950775146484</v>
+        <v>0.2557082176208496</v>
       </c>
       <c r="M13" t="n">
-        <v>9.041839001944167</v>
+        <v>8.91062527621914</v>
       </c>
       <c r="N13" t="n">
         <v>1.952922187827063e-07</v>
@@ -1343,58 +1343,58 @@
         <v>2</v>
       </c>
       <c r="H14" t="n">
-        <v>493.2969613259669</v>
+        <v>474.8406113537118</v>
       </c>
       <c r="I14" t="n">
-        <v>3.494417190551758</v>
+        <v>6.829186916351318</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="L14" t="n">
-        <v>0.06945204734802246</v>
+        <v>0.2205660343170166</v>
       </c>
       <c r="M14" t="n">
-        <v>50.31409906523448</v>
+        <v>30.96209685003367</v>
       </c>
       <c r="N14" t="n">
-        <v>4.108608584022105e-08</v>
+        <v>0.00158824764965587</v>
       </c>
       <c r="O14" t="n">
-        <v>0.02604806465610428</v>
+        <v>0.02595488759211882</v>
       </c>
       <c r="P14" t="n">
-        <v>0.9436274509803921</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.9305555555555556</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="R14" t="n">
-        <v>0.9434870906116276</v>
+        <v>0.958266450502248</v>
       </c>
       <c r="S14" t="n">
-        <v>0.9302938392054945</v>
+        <v>0.9410440911633036</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9436274509803921</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="U14" t="n">
-        <v>0.9305555555555556</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="V14" t="n">
-        <v>0.9440651169022576</v>
+        <v>0.9582971178249835</v>
       </c>
       <c r="W14" t="n">
-        <v>0.9319210201563143</v>
+        <v>0.9414496448734293</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9431234758054166</v>
+        <v>0.9582370684122705</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.9295822102425876</v>
+        <v>0.9407649852393787</v>
       </c>
     </row>
     <row r="15">
@@ -1422,10 +1422,10 @@
         <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>1336.691485809683</v>
+        <v>753.1784827059049</v>
       </c>
       <c r="I15" t="n">
-        <v>13.78874588012695</v>
+        <v>14.05977082252502</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
@@ -1434,10 +1434,10 @@
         <v>34</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2723519802093506</v>
+        <v>0.2785389423370361</v>
       </c>
       <c r="M15" t="n">
-        <v>50.62840325055785</v>
+        <v>50.47685865595231</v>
       </c>
       <c r="N15" t="n">
         <v>0.3026230227814357</v>

</xml_diff>

<commit_message>
fix(datasets): fix some path for the datasets
</commit_message>
<xml_diff>
--- a/hyperXGB/logs/all_datasets_comparison/comparison_results.xlsx
+++ b/hyperXGB/logs/all_datasets_comparison/comparison_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,22 +585,22 @@
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>186.6960269479135</v>
+        <v>180.2157904535495</v>
       </c>
       <c r="I2" t="n">
-        <v>31.60971188545227</v>
+        <v>31.78462314605713</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6250641345977783</v>
+        <v>0.634627103805542</v>
       </c>
       <c r="M2" t="n">
-        <v>50.57034972226132</v>
+        <v>50.08393583485579</v>
       </c>
       <c r="N2" t="n">
         <v>1.948093995367479e-07</v>
@@ -664,10 +664,10 @@
         <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>537.8993470910575</v>
+        <v>522.4041794310722</v>
       </c>
       <c r="I3" t="n">
-        <v>35.9458270072937</v>
+        <v>37.59940099716187</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -676,10 +676,10 @@
         <v>13</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6741127967834473</v>
+        <v>0.7027668952941895</v>
       </c>
       <c r="M3" t="n">
-        <v>53.32316368834781</v>
+        <v>53.50195242395724</v>
       </c>
       <c r="N3" t="n">
         <v>0.001579694065001903</v>
@@ -743,10 +743,10 @@
         <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>1594.280011506716</v>
+        <v>1548.273206461924</v>
       </c>
       <c r="I4" t="n">
-        <v>69.56055402755737</v>
+        <v>72.00728392601013</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -755,10 +755,10 @@
         <v>4</v>
       </c>
       <c r="L4" t="n">
-        <v>1.209961891174316</v>
+        <v>1.234483003616333</v>
       </c>
       <c r="M4" t="n">
-        <v>57.48987181740581</v>
+        <v>58.32991115719678</v>
       </c>
       <c r="N4" t="n">
         <v>0.3080625870352865</v>
@@ -822,10 +822,10 @@
         <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>49.41097724230254</v>
+        <v>47.23853211009175</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4972898960113525</v>
+        <v>0.4764890670776367</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -834,10 +834,10 @@
         <v>100</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2443199157714844</v>
+        <v>0.243311882019043</v>
       </c>
       <c r="M5" t="n">
-        <v>2.03540466376255</v>
+        <v>1.958346888461222</v>
       </c>
       <c r="N5" t="n">
         <v>8.590505752911891e-08</v>
@@ -901,10 +901,10 @@
         <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>138.1121856866538</v>
+        <v>167.5682656826568</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9521069526672363</v>
+        <v>0.9159867763519287</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -913,10 +913,10 @@
         <v>100</v>
       </c>
       <c r="L6" t="n">
-        <v>0.08733320236206055</v>
+        <v>0.08812284469604492</v>
       </c>
       <c r="M6" t="n">
-        <v>10.90200435706057</v>
+        <v>10.39443040577467</v>
       </c>
       <c r="N6" t="n">
         <v>0.001431014891680268</v>
@@ -980,10 +980,10 @@
         <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>406.3967264224473</v>
+        <v>510.6628256513026</v>
       </c>
       <c r="I7" t="n">
-        <v>5.503466844558716</v>
+        <v>5.37568998336792</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -992,10 +992,10 @@
         <v>100</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2481122016906738</v>
+        <v>0.2278590202331543</v>
       </c>
       <c r="M7" t="n">
-        <v>22.18136313755335</v>
+        <v>23.59217545071204</v>
       </c>
       <c r="N7" t="n">
         <v>0.2805947281718134</v>
@@ -1037,7 +1037,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ERROR</t>
+          <t>Logistic Regression</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1053,109 +1053,223 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
+        <v>115</v>
+      </c>
+      <c r="G8" t="n">
+        <v>12</v>
+      </c>
+      <c r="H8" t="n">
+        <v>136.0096153846154</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.812261819839478</v>
+      </c>
+      <c r="J8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.8971700668334961</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.019975795933249</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5.368833561089274e-09</v>
+      </c>
+      <c r="O8" t="n">
+        <v>8.913245851589174e-09</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.09502923976608187</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.09502923976608187</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.08962264150943396</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.08962264150943396</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ERROR</t>
+          <t>Poincare</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>UCIdataE</t>
+          <t>football</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>UCIdataE</t>
+          <t>football</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
+        <v>115</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12</v>
+      </c>
+      <c r="H9" t="n">
+        <v>435.736012608353</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.761344909667969</v>
+      </c>
+      <c r="J9" t="b">
         <v>0</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.3027389049530029</v>
+      </c>
+      <c r="M9" t="n">
+        <v>12.42438566081184</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.0005262370158466377</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.009382015461683255</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.0782608695652174</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.06956521739130435</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.02617079889807163</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.01084010840108401</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.0782608695652174</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.06956521739130435</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.04756637168141593</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.005797101449275362</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.0925925925925926</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.08333333333333333</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ERROR</t>
+          <t>Hyperboloid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>UCIdata</t>
+          <t>football</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UCIdata</t>
+          <t>football</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
+        <v>115</v>
+      </c>
+      <c r="G10" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1178.229066666667</v>
+      </c>
+      <c r="I10" t="n">
+        <v>22.72747707366943</v>
+      </c>
+      <c r="J10" t="b">
         <v>0</v>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.4988589286804199</v>
+      </c>
+      <c r="M10" t="n">
+        <v>45.55892611522076</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.2693482534015321</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.1546165185046081</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.1304347826086956</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.09502923976608187</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.05112044817927171</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.1478260869565217</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.1304347826086956</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.08962264150943396</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.03314814814814815</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.1469907407407407</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1165,12 +1279,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gauss</t>
+          <t>UCIdataE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>gauss</t>
+          <t>UCIdataE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1206,12 +1320,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>gausshyper</t>
+          <t>UCIdata</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>gausshyper</t>
+          <t>UCIdata</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1242,165 +1356,89 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Logistic Regression</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>polblogs</t>
+          <t>gauss</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>polblogs</t>
+          <t>gauss</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>1224</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" t="n">
-        <v>155.3291394061399</v>
-      </c>
-      <c r="I13" t="n">
-        <v>2.278520107269287</v>
-      </c>
-      <c r="J13" t="b">
         <v>0</v>
       </c>
-      <c r="K13" t="n">
-        <v>100</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.2557082176208496</v>
-      </c>
-      <c r="M13" t="n">
-        <v>8.91062527621914</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1.952922187827063e-07</v>
-      </c>
-      <c r="O13" t="n">
-        <v>3.177412159000643e-08</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0.9991830065359477</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.9991830065359477</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0.9991816951078871</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0.9991816951078871</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0.9991830065359477</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.9991830065359477</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0.999215070643642</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0.999215070643642</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0.9991496598639455</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>0.9991496598639455</v>
-      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Poincare</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>polblogs</t>
+          <t>gausshyper</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>polblogs</t>
+          <t>gausshyper</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>1224</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" t="n">
-        <v>474.8406113537118</v>
-      </c>
-      <c r="I14" t="n">
-        <v>6.829186916351318</v>
-      </c>
-      <c r="J14" t="b">
         <v>0</v>
       </c>
-      <c r="K14" t="n">
-        <v>100</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.2205660343170166</v>
-      </c>
-      <c r="M14" t="n">
-        <v>30.96209685003367</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.00158824764965587</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.02595488759211882</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0.9583333333333334</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.9411764705882353</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0.958266450502248</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.9410440911633036</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0.9583333333333334</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.9411764705882353</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0.9582971178249835</v>
-      </c>
-      <c r="W14" t="n">
-        <v>0.9414496448734293</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0.9582370684122705</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0.9407649852393787</v>
-      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hyperboloid</t>
+          <t>Logistic Regression</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1422,55 +1460,55 @@
         <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>753.1784827059049</v>
+        <v>198.8345370978332</v>
       </c>
       <c r="I15" t="n">
-        <v>14.05977082252502</v>
+        <v>2.279141902923584</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2785389423370361</v>
+        <v>0.2540719509124756</v>
       </c>
       <c r="M15" t="n">
-        <v>50.47685865595231</v>
+        <v>8.970458544275587</v>
       </c>
       <c r="N15" t="n">
-        <v>0.3026230227814357</v>
+        <v>1.952922187827063e-07</v>
       </c>
       <c r="O15" t="n">
-        <v>0.61993851553676</v>
+        <v>3.177412159000643e-08</v>
       </c>
       <c r="P15" t="n">
-        <v>0.9983660130718954</v>
+        <v>0.9991830065359477</v>
       </c>
       <c r="Q15" t="n">
         <v>0.9991830065359477</v>
       </c>
       <c r="R15" t="n">
-        <v>0.9983637019905618</v>
+        <v>0.9991816951078871</v>
       </c>
       <c r="S15" t="n">
         <v>0.9991816951078871</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9983660130718954</v>
+        <v>0.9991830065359477</v>
       </c>
       <c r="U15" t="n">
         <v>0.9991830065359477</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9983050847457627</v>
+        <v>0.999215070643642</v>
       </c>
       <c r="W15" t="n">
         <v>0.999215070643642</v>
       </c>
       <c r="X15" t="n">
-        <v>0.9984276729559749</v>
+        <v>0.9991496598639455</v>
       </c>
       <c r="Y15" t="n">
         <v>0.9991496598639455</v>
@@ -1479,43 +1517,397 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ERROR</t>
+          <t>Poincare</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>karate</t>
+          <t>polblogs</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>karate</t>
+          <t>polblogs</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
+        <v>1224</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>528.1431411530815</v>
+      </c>
+      <c r="I16" t="n">
+        <v>6.777577877044678</v>
+      </c>
+      <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.2235190868377686</v>
+      </c>
+      <c r="M16" t="n">
+        <v>30.3221437279935</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.00158824764965587</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.02595488759211882</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.9411764705882353</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.958266450502248</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.9410440911633036</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.9411764705882353</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.9582971178249835</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.9414496448734293</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.9582370684122705</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.9407649852393787</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hyperboloid</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>polblogs</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>polblogs</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>1224</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1320.543035279805</v>
+      </c>
+      <c r="I17" t="n">
+        <v>14.33179998397827</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="n">
+        <v>36</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.2804470062255859</v>
+      </c>
+      <c r="M17" t="n">
+        <v>51.10341585336825</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.3026230227814357</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.61993851553676</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.9983660130718954</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.9991830065359477</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.998363496341933</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.9991816951078871</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.9983660130718954</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.9991830065359477</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.998363496341933</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.999215070643642</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.998363496341933</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.9991496598639455</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Logistic Regression</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>34</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" t="n">
+        <v>19.75593952483802</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1456241607666016</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.09338498115539551</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.559395943168618</v>
+      </c>
+      <c r="N18" t="n">
+        <v>1.923327344684119e-07</v>
+      </c>
+      <c r="O18" t="n">
+        <v>3.416590174828492e-08</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1</v>
+      </c>
+      <c r="U18" t="n">
+        <v>1</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1</v>
+      </c>
+      <c r="X18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Poincare</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>34</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" t="n">
+        <v>46.48970588235294</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.245955228805542</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>100</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.05438375473022461</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4.522586386791874</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.001555222084127309</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.02652969078635097</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.9705882352941176</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.9705627705627706</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.9705882352941176</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.9722222222222222</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.9705882352941176</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Hyperboloid</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>34</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="n">
+        <v>169.9450464396285</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1.188036918640137</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>100</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.1515958309173584</v>
+      </c>
+      <c r="M20" t="n">
+        <v>7.836870654363762</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.3191324769816309</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.6262014968518443</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1</v>
+      </c>
+      <c r="T20" t="n">
+        <v>1</v>
+      </c>
+      <c r="U20" t="n">
+        <v>1</v>
+      </c>
+      <c r="V20" t="n">
+        <v>1</v>
+      </c>
+      <c r="W20" t="n">
+        <v>1</v>
+      </c>
+      <c r="X20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>